<commit_message>
Added tests for responsive testing for PageOptions
</commit_message>
<xml_diff>
--- a/test-data/page-options-data.xlsx
+++ b/test-data/page-options-data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE7866F-13AB-4F3C-B4E4-F54739FC2A4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B306679-6CDA-4949-9869-B9264402B17C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_pageoptions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
   <si>
     <t>path</t>
   </si>
@@ -64,6 +64,30 @@
   </si>
   <si>
     <t>Event</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/side-effects/fatigue/fatigue-pdq</t>
+  </si>
+  <si>
+    <t>PDQ Cancer Information Summary</t>
+  </si>
+  <si>
+    <t>/espanol/cancer/tratamiento/efectos-secundarios/fatiga/fatiga-pdq</t>
+  </si>
+  <si>
+    <t>/about-cancer</t>
+  </si>
+  <si>
+    <t>Home &amp; Landing</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/drugs/bevacizumab</t>
+  </si>
+  <si>
+    <t>PDQ Drug Information Summary</t>
+  </si>
+  <si>
+    <t>/espanol/tipos</t>
   </si>
 </sst>
 </file>
@@ -393,13 +417,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.5703125" customWidth="1"/>
+    <col min="1" max="1" width="62" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -496,41 +521,103 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{887321EA-66E5-437B-9E82-0613112B40E5}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550C9103-3B9D-4803-8025-F0900931F8E9}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="52.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -544,6 +631,61 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Introduced the use of ElementHelper class
</commit_message>
<xml_diff>
--- a/test-data/page-options-data.xlsx
+++ b/test-data/page-options-data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B306679-6CDA-4949-9869-B9264402B17C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F095E312-B09E-401B-9E01-ED0042658FD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_pageoptions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="20">
   <si>
     <t>path</t>
   </si>
@@ -79,12 +79,6 @@
   </si>
   <si>
     <t>Home &amp; Landing</t>
-  </si>
-  <si>
-    <t>/about-cancer/treatment/drugs/bevacizumab</t>
-  </si>
-  <si>
-    <t>PDQ Drug Information Summary</t>
   </si>
   <si>
     <t>/espanol/tipos</t>
@@ -417,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,10 +515,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{887321EA-66E5-437B-9E82-0613112B40E5}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,17 +583,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -610,13 +593,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550C9103-3B9D-4803-8025-F0900931F8E9}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.42578125" customWidth="1"/>
+    <col min="1" max="1" width="61.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -677,7 +660,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>

</xml_diff>